<commit_message>
fixed bug related to depth tracker and the stack dictionary
</commit_message>
<xml_diff>
--- a/xword_grid.xlsx
+++ b/xword_grid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakes\Documents\R\xword-generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jse/Documents/R_proj/xword-generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F9ADCE-3A8F-49C6-BCB9-91B065CAAC70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6265A9B-3B6D-7748-9836-D49DDB6084ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5610" yWindow="3190" windowWidth="22590" windowHeight="15430" xr2:uid="{8DDEDC45-C5AF-4FCB-9BF3-9FD08DEC95AE}"/>
+    <workbookView xWindow="5620" yWindow="1100" windowWidth="22600" windowHeight="15440" xr2:uid="{8DDEDC45-C5AF-4FCB-9BF3-9FD08DEC95AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="1">
   <si>
     <t>?</t>
   </si>
@@ -52,18 +51,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -78,9 +71,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,22 +387,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18BF09C-66F4-44FF-B0A3-23DD0E125386}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="15" width="2.7265625" customWidth="1"/>
-    <col min="16" max="20" width="3.26953125" customWidth="1"/>
+    <col min="1" max="15" width="2.6640625" customWidth="1"/>
+    <col min="16" max="20" width="3.33203125" customWidth="1"/>
     <col min="21" max="51" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -420,11 +416,11 @@
       <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -437,12 +433,8 @@
       <c r="E2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -458,14 +450,8 @@
       <c r="E3" t="s">
         <v>0</v>
       </c>
-      <c r="F3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -481,14 +467,8 @@
       <c r="E4" t="s">
         <v>0</v>
       </c>
-      <c r="F4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -504,46 +484,6 @@
       <c r="E5" t="s">
         <v>0</v>
       </c>
-      <c r="F5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Still broken, about to make a big change: will jump to the earliest affected position and insert random words to guard against repeating the same failure
</commit_message>
<xml_diff>
--- a/xword_grid.xlsx
+++ b/xword_grid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jse/Documents/R_proj/xword-generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2DFE0F-EBF3-A04A-87B4-2527E3A86F51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAD85D0-0FEC-3E42-9EE7-83AC70A06F9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16080" xr2:uid="{8DDEDC45-C5AF-4FCB-9BF3-9FD08DEC95AE}"/>
   </bookViews>
@@ -397,7 +397,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Random word is now chosen to populate puzzle to avoid getting hung up on a single bad word
</commit_message>
<xml_diff>
--- a/xword_grid.xlsx
+++ b/xword_grid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jse/Documents/R_proj/xword-generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAD85D0-0FEC-3E42-9EE7-83AC70A06F9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11893775-5668-B448-98DE-6CEBDDC050CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16080" xr2:uid="{8DDEDC45-C5AF-4FCB-9BF3-9FD08DEC95AE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="1">
   <si>
     <t>?</t>
   </si>
@@ -394,20 +394,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18BF09C-66F4-44FF-B0A3-23DD0E125386}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:AD30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="15" width="2.6640625" customWidth="1"/>
-    <col min="16" max="20" width="3.33203125" customWidth="1"/>
-    <col min="21" max="51" width="3" customWidth="1"/>
+    <col min="1" max="30" width="2.5" customWidth="1"/>
+    <col min="31" max="51" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -417,10 +416,10 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1"/>
       <c r="F1" t="s">
         <v>0</v>
       </c>
@@ -433,10 +432,10 @@
       <c r="I1" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" t="s">
-        <v>0</v>
-      </c>
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1"/>
       <c r="L1" t="s">
         <v>0</v>
       </c>
@@ -449,8 +448,49 @@
       <c r="O1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T1" s="1"/>
+      <c r="U1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z1" s="1"/>
+      <c r="AA1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -460,10 +500,10 @@
       <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" t="s">
-        <v>0</v>
-      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1"/>
       <c r="F2" t="s">
         <v>0</v>
       </c>
@@ -473,13 +513,13 @@
       <c r="H2" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="1"/>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
       <c r="J2" t="s">
         <v>0</v>
       </c>
-      <c r="K2" t="s">
-        <v>0</v>
-      </c>
+      <c r="K2" s="1"/>
       <c r="L2" t="s">
         <v>0</v>
       </c>
@@ -492,8 +532,49 @@
       <c r="O2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1"/>
+      <c r="U2" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" t="s">
+        <v>0</v>
+      </c>
+      <c r="W2" t="s">
+        <v>0</v>
+      </c>
+      <c r="X2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="1"/>
+      <c r="AA2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -503,10 +584,10 @@
       <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1"/>
       <c r="F3" t="s">
         <v>0</v>
       </c>
@@ -516,13 +597,13 @@
       <c r="H3" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="I3" t="s">
+        <v>0</v>
+      </c>
       <c r="J3" t="s">
         <v>0</v>
       </c>
-      <c r="K3" t="s">
-        <v>0</v>
-      </c>
+      <c r="K3" s="1"/>
       <c r="L3" t="s">
         <v>0</v>
       </c>
@@ -535,18 +616,59 @@
       <c r="O3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
+      <c r="P3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>0</v>
+      </c>
+      <c r="R3" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" t="s">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1"/>
+      <c r="U3" t="s">
+        <v>0</v>
+      </c>
+      <c r="V3" t="s">
+        <v>0</v>
+      </c>
+      <c r="W3" t="s">
+        <v>0</v>
+      </c>
+      <c r="X3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="1"/>
+      <c r="AA3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
-        <v>0</v>
-      </c>
+      <c r="D4" s="1"/>
       <c r="E4" t="s">
         <v>0</v>
       </c>
@@ -556,24 +678,71 @@
       <c r="G4" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" t="s">
+        <v>0</v>
+      </c>
       <c r="I4" t="s">
         <v>0</v>
       </c>
-      <c r="J4" t="s">
-        <v>0</v>
-      </c>
+      <c r="J4" s="1"/>
       <c r="K4" t="s">
         <v>0</v>
       </c>
       <c r="L4" t="s">
         <v>0</v>
       </c>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1"/>
+      <c r="T4" t="s">
+        <v>0</v>
+      </c>
+      <c r="U4" t="s">
+        <v>0</v>
+      </c>
+      <c r="V4" t="s">
+        <v>0</v>
+      </c>
+      <c r="W4" t="s">
+        <v>0</v>
+      </c>
+      <c r="X4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="1"/>
+      <c r="Z4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -586,19 +755,17 @@
       <c r="D5" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
       <c r="F5" t="s">
         <v>0</v>
       </c>
       <c r="G5" t="s">
         <v>0</v>
       </c>
-      <c r="H5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I5" t="s">
-        <v>0</v>
-      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
       <c r="J5" t="s">
         <v>0</v>
       </c>
@@ -608,36 +775,59 @@
       <c r="L5" t="s">
         <v>0</v>
       </c>
-      <c r="M5" t="s">
-        <v>0</v>
-      </c>
-      <c r="N5" t="s">
-        <v>0</v>
-      </c>
-      <c r="O5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>0</v>
+      </c>
+      <c r="R5" t="s">
+        <v>0</v>
+      </c>
+      <c r="S5" t="s">
+        <v>0</v>
+      </c>
+      <c r="T5" t="s">
+        <v>0</v>
+      </c>
+      <c r="U5" t="s">
+        <v>0</v>
+      </c>
+      <c r="V5" t="s">
+        <v>0</v>
+      </c>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
       <c r="D6" t="s">
         <v>0</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" t="s">
-        <v>0</v>
-      </c>
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1"/>
       <c r="H6" t="s">
         <v>0</v>
       </c>
@@ -647,7 +837,9 @@
       <c r="J6" t="s">
         <v>0</v>
       </c>
-      <c r="K6" s="1"/>
+      <c r="K6" t="s">
+        <v>0</v>
+      </c>
       <c r="L6" t="s">
         <v>0</v>
       </c>
@@ -660,21 +852,62 @@
       <c r="O6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T6" t="s">
+        <v>0</v>
+      </c>
+      <c r="U6" t="s">
+        <v>0</v>
+      </c>
+      <c r="V6" s="1"/>
+      <c r="W6" t="s">
+        <v>0</v>
+      </c>
+      <c r="X6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
       <c r="D7" t="s">
         <v>0</v>
       </c>
-      <c r="E7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
       <c r="H7" t="s">
         <v>0</v>
       </c>
@@ -697,18 +930,57 @@
       <c r="O7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
+      <c r="P7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>0</v>
+      </c>
+      <c r="R7" t="s">
+        <v>0</v>
+      </c>
+      <c r="S7" t="s">
+        <v>0</v>
+      </c>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" t="s">
+        <v>0</v>
+      </c>
+      <c r="W7" t="s">
+        <v>0</v>
+      </c>
+      <c r="X7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="1"/>
+      <c r="AB7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
       <c r="B8" t="s">
         <v>0</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
       </c>
-      <c r="D8" t="s">
-        <v>0</v>
-      </c>
+      <c r="D8" s="1"/>
       <c r="E8" t="s">
         <v>0</v>
       </c>
@@ -718,7 +990,9 @@
       <c r="G8" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="1"/>
+      <c r="H8" t="s">
+        <v>0</v>
+      </c>
       <c r="I8" t="s">
         <v>0</v>
       </c>
@@ -728,18 +1002,59 @@
       <c r="K8" t="s">
         <v>0</v>
       </c>
-      <c r="L8" t="s">
-        <v>0</v>
-      </c>
+      <c r="L8" s="1"/>
       <c r="M8" t="s">
         <v>0</v>
       </c>
       <c r="N8" t="s">
         <v>0</v>
       </c>
-      <c r="O8" s="1"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O8" t="s">
+        <v>0</v>
+      </c>
+      <c r="P8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R8" t="s">
+        <v>0</v>
+      </c>
+      <c r="S8" s="1"/>
+      <c r="T8" t="s">
+        <v>0</v>
+      </c>
+      <c r="U8" t="s">
+        <v>0</v>
+      </c>
+      <c r="V8" t="s">
+        <v>0</v>
+      </c>
+      <c r="W8" t="s">
+        <v>0</v>
+      </c>
+      <c r="X8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="1"/>
+      <c r="AB8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -762,21 +1077,64 @@
       <c r="H9" t="s">
         <v>0</v>
       </c>
-      <c r="I9" s="1"/>
-      <c r="J9" t="s">
-        <v>0</v>
-      </c>
-      <c r="K9" t="s">
-        <v>0</v>
-      </c>
+      <c r="I9" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
       <c r="L9" t="s">
         <v>0</v>
       </c>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M9" t="s">
+        <v>0</v>
+      </c>
+      <c r="N9" t="s">
+        <v>0</v>
+      </c>
+      <c r="O9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>0</v>
+      </c>
+      <c r="R9" t="s">
+        <v>0</v>
+      </c>
+      <c r="S9" s="1"/>
+      <c r="T9" t="s">
+        <v>0</v>
+      </c>
+      <c r="U9" t="s">
+        <v>0</v>
+      </c>
+      <c r="V9" t="s">
+        <v>0</v>
+      </c>
+      <c r="W9" t="s">
+        <v>0</v>
+      </c>
+      <c r="X9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -789,7 +1147,9 @@
       <c r="D10" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" t="s">
+        <v>0</v>
+      </c>
       <c r="F10" t="s">
         <v>0</v>
       </c>
@@ -799,36 +1159,61 @@
       <c r="H10" t="s">
         <v>0</v>
       </c>
-      <c r="I10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" t="s">
+        <v>0</v>
+      </c>
       <c r="K10" t="s">
         <v>0</v>
       </c>
       <c r="L10" t="s">
         <v>0</v>
       </c>
-      <c r="M10" t="s">
-        <v>0</v>
-      </c>
-      <c r="N10" t="s">
-        <v>0</v>
-      </c>
-      <c r="O10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" t="s">
-        <v>0</v>
-      </c>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>0</v>
+      </c>
+      <c r="R10" t="s">
+        <v>0</v>
+      </c>
+      <c r="S10" t="s">
+        <v>0</v>
+      </c>
+      <c r="T10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U10" t="s">
+        <v>0</v>
+      </c>
+      <c r="V10" t="s">
+        <v>0</v>
+      </c>
+      <c r="W10" t="s">
+        <v>0</v>
+      </c>
+      <c r="X10" s="1"/>
+      <c r="Y10" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
       <c r="D11" t="s">
         <v>0</v>
       </c>
@@ -838,19 +1223,17 @@
       <c r="F11" t="s">
         <v>0</v>
       </c>
-      <c r="G11" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" t="s">
-        <v>0</v>
-      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
       <c r="I11" t="s">
         <v>0</v>
       </c>
       <c r="J11" t="s">
         <v>0</v>
       </c>
-      <c r="K11" s="1"/>
+      <c r="K11" t="s">
+        <v>0</v>
+      </c>
       <c r="L11" t="s">
         <v>0</v>
       </c>
@@ -863,24 +1246,65 @@
       <c r="O11" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" t="s">
+        <v>0</v>
+      </c>
+      <c r="T11" t="s">
+        <v>0</v>
+      </c>
+      <c r="U11" t="s">
+        <v>0</v>
+      </c>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
       <c r="D12" t="s">
         <v>0</v>
       </c>
       <c r="E12" t="s">
         <v>0</v>
       </c>
-      <c r="F12" t="s">
-        <v>0</v>
-      </c>
+      <c r="F12" s="1"/>
       <c r="G12" t="s">
         <v>0</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" t="s">
+        <v>0</v>
+      </c>
       <c r="I12" t="s">
         <v>0</v>
       </c>
@@ -890,18 +1314,59 @@
       <c r="K12" t="s">
         <v>0</v>
       </c>
-      <c r="L12" t="s">
-        <v>0</v>
-      </c>
+      <c r="L12" s="1"/>
       <c r="M12" t="s">
         <v>0</v>
       </c>
       <c r="N12" t="s">
         <v>0</v>
       </c>
-      <c r="O12" s="1"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O12" t="s">
+        <v>0</v>
+      </c>
+      <c r="P12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S12" t="s">
+        <v>0</v>
+      </c>
+      <c r="T12" t="s">
+        <v>0</v>
+      </c>
+      <c r="U12" s="1"/>
+      <c r="V12" t="s">
+        <v>0</v>
+      </c>
+      <c r="W12" t="s">
+        <v>0</v>
+      </c>
+      <c r="X12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="1"/>
+      <c r="AB12" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -914,13 +1379,13 @@
       <c r="D13" t="s">
         <v>0</v>
       </c>
-      <c r="E13" t="s">
-        <v>0</v>
-      </c>
+      <c r="E13" s="1"/>
       <c r="F13" t="s">
         <v>0</v>
       </c>
-      <c r="G13" s="1"/>
+      <c r="G13" t="s">
+        <v>0</v>
+      </c>
       <c r="H13" t="s">
         <v>0</v>
       </c>
@@ -930,10 +1395,10 @@
       <c r="J13" t="s">
         <v>0</v>
       </c>
-      <c r="K13" t="s">
-        <v>0</v>
-      </c>
-      <c r="L13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" t="s">
+        <v>0</v>
+      </c>
       <c r="M13" t="s">
         <v>0</v>
       </c>
@@ -943,8 +1408,49 @@
       <c r="O13" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R13" t="s">
+        <v>0</v>
+      </c>
+      <c r="S13" t="s">
+        <v>0</v>
+      </c>
+      <c r="T13" s="1"/>
+      <c r="U13" t="s">
+        <v>0</v>
+      </c>
+      <c r="V13" t="s">
+        <v>0</v>
+      </c>
+      <c r="W13" t="s">
+        <v>0</v>
+      </c>
+      <c r="X13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="1"/>
+      <c r="AA13" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -957,13 +1463,13 @@
       <c r="D14" t="s">
         <v>0</v>
       </c>
-      <c r="E14" t="s">
-        <v>0</v>
-      </c>
+      <c r="E14" s="1"/>
       <c r="F14" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="1"/>
+      <c r="G14" t="s">
+        <v>0</v>
+      </c>
       <c r="H14" t="s">
         <v>0</v>
       </c>
@@ -973,10 +1479,10 @@
       <c r="J14" t="s">
         <v>0</v>
       </c>
-      <c r="K14" t="s">
-        <v>0</v>
-      </c>
-      <c r="L14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" t="s">
+        <v>0</v>
+      </c>
       <c r="M14" t="s">
         <v>0</v>
       </c>
@@ -986,8 +1492,49 @@
       <c r="O14" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P14" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>0</v>
+      </c>
+      <c r="R14" t="s">
+        <v>0</v>
+      </c>
+      <c r="S14" t="s">
+        <v>0</v>
+      </c>
+      <c r="T14" s="1"/>
+      <c r="U14" t="s">
+        <v>0</v>
+      </c>
+      <c r="V14" t="s">
+        <v>0</v>
+      </c>
+      <c r="W14" t="s">
+        <v>0</v>
+      </c>
+      <c r="X14" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="1"/>
+      <c r="AA14" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1000,10 +1547,10 @@
       <c r="D15" t="s">
         <v>0</v>
       </c>
-      <c r="E15" t="s">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" t="s">
+        <v>0</v>
+      </c>
       <c r="G15" t="s">
         <v>0</v>
       </c>
@@ -1016,17 +1563,1262 @@
       <c r="J15" t="s">
         <v>0</v>
       </c>
-      <c r="K15" t="s">
-        <v>0</v>
-      </c>
-      <c r="L15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" t="s">
+        <v>0</v>
+      </c>
       <c r="M15" t="s">
         <v>0</v>
       </c>
       <c r="N15" t="s">
         <v>0</v>
       </c>
-      <c r="O15" t="s">
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" t="s">
+        <v>0</v>
+      </c>
+      <c r="R15" t="s">
+        <v>0</v>
+      </c>
+      <c r="S15" t="s">
+        <v>0</v>
+      </c>
+      <c r="T15" s="1"/>
+      <c r="U15" t="s">
+        <v>0</v>
+      </c>
+      <c r="V15" t="s">
+        <v>0</v>
+      </c>
+      <c r="W15" t="s">
+        <v>0</v>
+      </c>
+      <c r="X15" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="1"/>
+      <c r="AA15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1"/>
+      <c r="L16" t="s">
+        <v>0</v>
+      </c>
+      <c r="M16" t="s">
+        <v>0</v>
+      </c>
+      <c r="N16" t="s">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" t="s">
+        <v>0</v>
+      </c>
+      <c r="R16" t="s">
+        <v>0</v>
+      </c>
+      <c r="S16" t="s">
+        <v>0</v>
+      </c>
+      <c r="T16" s="1"/>
+      <c r="U16" t="s">
+        <v>0</v>
+      </c>
+      <c r="V16" t="s">
+        <v>0</v>
+      </c>
+      <c r="W16" t="s">
+        <v>0</v>
+      </c>
+      <c r="X16" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="1"/>
+      <c r="AA16" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1"/>
+      <c r="L17" t="s">
+        <v>0</v>
+      </c>
+      <c r="M17" t="s">
+        <v>0</v>
+      </c>
+      <c r="N17" t="s">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
+        <v>0</v>
+      </c>
+      <c r="P17" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>0</v>
+      </c>
+      <c r="R17" t="s">
+        <v>0</v>
+      </c>
+      <c r="S17" t="s">
+        <v>0</v>
+      </c>
+      <c r="T17" s="1"/>
+      <c r="U17" t="s">
+        <v>0</v>
+      </c>
+      <c r="V17" t="s">
+        <v>0</v>
+      </c>
+      <c r="W17" t="s">
+        <v>0</v>
+      </c>
+      <c r="X17" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="1"/>
+      <c r="AA17" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" t="s">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1"/>
+      <c r="L18" t="s">
+        <v>0</v>
+      </c>
+      <c r="M18" t="s">
+        <v>0</v>
+      </c>
+      <c r="N18" t="s">
+        <v>0</v>
+      </c>
+      <c r="O18" t="s">
+        <v>0</v>
+      </c>
+      <c r="P18" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>0</v>
+      </c>
+      <c r="R18" t="s">
+        <v>0</v>
+      </c>
+      <c r="S18" t="s">
+        <v>0</v>
+      </c>
+      <c r="T18" s="1"/>
+      <c r="U18" t="s">
+        <v>0</v>
+      </c>
+      <c r="V18" t="s">
+        <v>0</v>
+      </c>
+      <c r="W18" t="s">
+        <v>0</v>
+      </c>
+      <c r="X18" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="1"/>
+      <c r="AA18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" t="s">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1"/>
+      <c r="K19" t="s">
+        <v>0</v>
+      </c>
+      <c r="L19" t="s">
+        <v>0</v>
+      </c>
+      <c r="M19" t="s">
+        <v>0</v>
+      </c>
+      <c r="N19" t="s">
+        <v>0</v>
+      </c>
+      <c r="O19" t="s">
+        <v>0</v>
+      </c>
+      <c r="P19" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>0</v>
+      </c>
+      <c r="R19" t="s">
+        <v>0</v>
+      </c>
+      <c r="S19" s="1"/>
+      <c r="T19" t="s">
+        <v>0</v>
+      </c>
+      <c r="U19" t="s">
+        <v>0</v>
+      </c>
+      <c r="V19" t="s">
+        <v>0</v>
+      </c>
+      <c r="W19" t="s">
+        <v>0</v>
+      </c>
+      <c r="X19" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="1"/>
+      <c r="Z19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" t="s">
+        <v>0</v>
+      </c>
+      <c r="K20" t="s">
+        <v>0</v>
+      </c>
+      <c r="L20" t="s">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>0</v>
+      </c>
+      <c r="R20" t="s">
+        <v>0</v>
+      </c>
+      <c r="S20" t="s">
+        <v>0</v>
+      </c>
+      <c r="T20" t="s">
+        <v>0</v>
+      </c>
+      <c r="U20" t="s">
+        <v>0</v>
+      </c>
+      <c r="V20" t="s">
+        <v>0</v>
+      </c>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1"/>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" t="s">
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>0</v>
+      </c>
+      <c r="J21" t="s">
+        <v>0</v>
+      </c>
+      <c r="K21" t="s">
+        <v>0</v>
+      </c>
+      <c r="L21" t="s">
+        <v>0</v>
+      </c>
+      <c r="M21" t="s">
+        <v>0</v>
+      </c>
+      <c r="N21" t="s">
+        <v>0</v>
+      </c>
+      <c r="O21" t="s">
+        <v>0</v>
+      </c>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" t="s">
+        <v>0</v>
+      </c>
+      <c r="T21" t="s">
+        <v>0</v>
+      </c>
+      <c r="U21" t="s">
+        <v>0</v>
+      </c>
+      <c r="V21" s="1"/>
+      <c r="W21" t="s">
+        <v>0</v>
+      </c>
+      <c r="X21" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>0</v>
+      </c>
+      <c r="J22" t="s">
+        <v>0</v>
+      </c>
+      <c r="K22" t="s">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1"/>
+      <c r="M22" t="s">
+        <v>0</v>
+      </c>
+      <c r="N22" t="s">
+        <v>0</v>
+      </c>
+      <c r="O22" t="s">
+        <v>0</v>
+      </c>
+      <c r="P22" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>0</v>
+      </c>
+      <c r="R22" t="s">
+        <v>0</v>
+      </c>
+      <c r="S22" t="s">
+        <v>0</v>
+      </c>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" t="s">
+        <v>0</v>
+      </c>
+      <c r="W22" t="s">
+        <v>0</v>
+      </c>
+      <c r="X22" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="1"/>
+      <c r="AB22" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" t="s">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>0</v>
+      </c>
+      <c r="J23" t="s">
+        <v>0</v>
+      </c>
+      <c r="K23" t="s">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1"/>
+      <c r="M23" t="s">
+        <v>0</v>
+      </c>
+      <c r="N23" t="s">
+        <v>0</v>
+      </c>
+      <c r="O23" t="s">
+        <v>0</v>
+      </c>
+      <c r="P23" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>0</v>
+      </c>
+      <c r="R23" t="s">
+        <v>0</v>
+      </c>
+      <c r="S23" s="1"/>
+      <c r="T23" t="s">
+        <v>0</v>
+      </c>
+      <c r="U23" t="s">
+        <v>0</v>
+      </c>
+      <c r="V23" t="s">
+        <v>0</v>
+      </c>
+      <c r="W23" t="s">
+        <v>0</v>
+      </c>
+      <c r="X23" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="1"/>
+      <c r="AB23" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>0</v>
+      </c>
+      <c r="G24" t="s">
+        <v>0</v>
+      </c>
+      <c r="H24" t="s">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>0</v>
+      </c>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" t="s">
+        <v>0</v>
+      </c>
+      <c r="M24" t="s">
+        <v>0</v>
+      </c>
+      <c r="N24" t="s">
+        <v>0</v>
+      </c>
+      <c r="O24" t="s">
+        <v>0</v>
+      </c>
+      <c r="P24" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>0</v>
+      </c>
+      <c r="R24" t="s">
+        <v>0</v>
+      </c>
+      <c r="S24" s="1"/>
+      <c r="T24" t="s">
+        <v>0</v>
+      </c>
+      <c r="U24" t="s">
+        <v>0</v>
+      </c>
+      <c r="V24" t="s">
+        <v>0</v>
+      </c>
+      <c r="W24" t="s">
+        <v>0</v>
+      </c>
+      <c r="X24" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1"/>
+      <c r="J25" t="s">
+        <v>0</v>
+      </c>
+      <c r="K25" t="s">
+        <v>0</v>
+      </c>
+      <c r="L25" t="s">
+        <v>0</v>
+      </c>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>0</v>
+      </c>
+      <c r="R25" t="s">
+        <v>0</v>
+      </c>
+      <c r="S25" t="s">
+        <v>0</v>
+      </c>
+      <c r="T25" t="s">
+        <v>0</v>
+      </c>
+      <c r="U25" t="s">
+        <v>0</v>
+      </c>
+      <c r="V25" t="s">
+        <v>0</v>
+      </c>
+      <c r="W25" t="s">
+        <v>0</v>
+      </c>
+      <c r="X25" s="1"/>
+      <c r="Y25" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="1"/>
+      <c r="AC25" s="1"/>
+      <c r="AD25" s="1"/>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" t="s">
+        <v>0</v>
+      </c>
+      <c r="J26" t="s">
+        <v>0</v>
+      </c>
+      <c r="K26" t="s">
+        <v>0</v>
+      </c>
+      <c r="L26" t="s">
+        <v>0</v>
+      </c>
+      <c r="M26" t="s">
+        <v>0</v>
+      </c>
+      <c r="N26" t="s">
+        <v>0</v>
+      </c>
+      <c r="O26" t="s">
+        <v>0</v>
+      </c>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" t="s">
+        <v>0</v>
+      </c>
+      <c r="T26" t="s">
+        <v>0</v>
+      </c>
+      <c r="U26" t="s">
+        <v>0</v>
+      </c>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" t="s">
+        <v>0</v>
+      </c>
+      <c r="H27" t="s">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
+        <v>0</v>
+      </c>
+      <c r="J27" t="s">
+        <v>0</v>
+      </c>
+      <c r="K27" t="s">
+        <v>0</v>
+      </c>
+      <c r="L27" s="1"/>
+      <c r="M27" t="s">
+        <v>0</v>
+      </c>
+      <c r="N27" t="s">
+        <v>0</v>
+      </c>
+      <c r="O27" t="s">
+        <v>0</v>
+      </c>
+      <c r="P27" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>0</v>
+      </c>
+      <c r="R27" t="s">
+        <v>0</v>
+      </c>
+      <c r="S27" t="s">
+        <v>0</v>
+      </c>
+      <c r="T27" t="s">
+        <v>0</v>
+      </c>
+      <c r="U27" s="1"/>
+      <c r="V27" t="s">
+        <v>0</v>
+      </c>
+      <c r="W27" t="s">
+        <v>0</v>
+      </c>
+      <c r="X27" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="1"/>
+      <c r="AB27" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" t="s">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>0</v>
+      </c>
+      <c r="J28" t="s">
+        <v>0</v>
+      </c>
+      <c r="K28" s="1"/>
+      <c r="L28" t="s">
+        <v>0</v>
+      </c>
+      <c r="M28" t="s">
+        <v>0</v>
+      </c>
+      <c r="N28" t="s">
+        <v>0</v>
+      </c>
+      <c r="O28" t="s">
+        <v>0</v>
+      </c>
+      <c r="P28" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>0</v>
+      </c>
+      <c r="R28" t="s">
+        <v>0</v>
+      </c>
+      <c r="S28" t="s">
+        <v>0</v>
+      </c>
+      <c r="T28" s="1"/>
+      <c r="U28" t="s">
+        <v>0</v>
+      </c>
+      <c r="V28" t="s">
+        <v>0</v>
+      </c>
+      <c r="W28" t="s">
+        <v>0</v>
+      </c>
+      <c r="X28" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="1"/>
+      <c r="AA28" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H29" t="s">
+        <v>0</v>
+      </c>
+      <c r="I29" t="s">
+        <v>0</v>
+      </c>
+      <c r="J29" t="s">
+        <v>0</v>
+      </c>
+      <c r="K29" s="1"/>
+      <c r="L29" t="s">
+        <v>0</v>
+      </c>
+      <c r="M29" t="s">
+        <v>0</v>
+      </c>
+      <c r="N29" t="s">
+        <v>0</v>
+      </c>
+      <c r="O29" t="s">
+        <v>0</v>
+      </c>
+      <c r="P29" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>0</v>
+      </c>
+      <c r="R29" t="s">
+        <v>0</v>
+      </c>
+      <c r="S29" t="s">
+        <v>0</v>
+      </c>
+      <c r="T29" s="1"/>
+      <c r="U29" t="s">
+        <v>0</v>
+      </c>
+      <c r="V29" t="s">
+        <v>0</v>
+      </c>
+      <c r="W29" t="s">
+        <v>0</v>
+      </c>
+      <c r="X29" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="1"/>
+      <c r="AA29" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" t="s">
+        <v>0</v>
+      </c>
+      <c r="G30" t="s">
+        <v>0</v>
+      </c>
+      <c r="H30" t="s">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
+        <v>0</v>
+      </c>
+      <c r="J30" t="s">
+        <v>0</v>
+      </c>
+      <c r="K30" s="1"/>
+      <c r="L30" t="s">
+        <v>0</v>
+      </c>
+      <c r="M30" t="s">
+        <v>0</v>
+      </c>
+      <c r="N30" t="s">
+        <v>0</v>
+      </c>
+      <c r="O30" t="s">
+        <v>0</v>
+      </c>
+      <c r="P30" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>0</v>
+      </c>
+      <c r="R30" t="s">
+        <v>0</v>
+      </c>
+      <c r="S30" t="s">
+        <v>0</v>
+      </c>
+      <c r="T30" s="1"/>
+      <c r="U30" t="s">
+        <v>0</v>
+      </c>
+      <c r="V30" t="s">
+        <v>0</v>
+      </c>
+      <c r="W30" t="s">
+        <v>0</v>
+      </c>
+      <c r="X30" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z30" s="1"/>
+      <c r="AA30" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD30" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>